<commit_message>
visual for f1 change over rfe and fix u2r roc
</commit_message>
<xml_diff>
--- a/visuals_u2r_attack_length_stats.xlsx
+++ b/visuals_u2r_attack_length_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casey\Documents\GitHub\ids_svm_slidingwindow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ids_svm_slidingwindow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D48B17B-FD06-4A74-920B-4178B67C8AD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38935624-3F50-469F-9EBB-811F91B50076}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12CF8178-9708-4750-A748-3ECF2E8290DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12CF8178-9708-4750-A748-3ECF2E8290DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,36 +42,6 @@
     <t>Actual Numbers</t>
   </si>
   <si>
-    <t>8 out of 18</t>
-  </si>
-  <si>
-    <t>8 out of 16</t>
-  </si>
-  <si>
-    <t>8 out of 15</t>
-  </si>
-  <si>
-    <t>7 out of 13</t>
-  </si>
-  <si>
-    <t>6 out of 12</t>
-  </si>
-  <si>
-    <t>6 out of 11</t>
-  </si>
-  <si>
-    <t>2 out of 7</t>
-  </si>
-  <si>
-    <t>2 out of 5</t>
-  </si>
-  <si>
-    <t>1 out of 3</t>
-  </si>
-  <si>
-    <t>0 out of 1</t>
-  </si>
-  <si>
     <t>Attack Length</t>
   </si>
   <si>
@@ -82,6 +52,36 @@
   </si>
   <si>
     <t>Predicted Positive Rate</t>
+  </si>
+  <si>
+    <t>10 out of 19</t>
+  </si>
+  <si>
+    <t>10 out of 17</t>
+  </si>
+  <si>
+    <t>10 out of 16</t>
+  </si>
+  <si>
+    <t>9 out of 14</t>
+  </si>
+  <si>
+    <t>8 out of 13</t>
+  </si>
+  <si>
+    <t>8 out of 12</t>
+  </si>
+  <si>
+    <t>4 out of 8</t>
+  </si>
+  <si>
+    <t>4 out of 6</t>
+  </si>
+  <si>
+    <t>3 out of 4</t>
+  </si>
+  <si>
+    <t>1 out of 1</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs Classification ROC</a:t>
+              <a:t> Threshold vs Classification</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -289,34 +289,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.44444444444444442</c:v>
+                  <c:v>0.52631578947368418</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.58823529411764708</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61538461538461542</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.53333333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.53846153846153844</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.54545454545454541</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.2857142857142857</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,6 +451,7 @@
         <c:axId val="722559080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3521,18 +3522,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7C606F-D4FB-4A67-BDC6-9C4152EF9960}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3543,34 +3544,37 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2">
-        <f>8/18</f>
-        <v>0.44444444444444442</v>
+        <f>10/19</f>
+        <v>0.52631578947368418</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>2766</v>
@@ -3582,6 +3586,9 @@
         <f>PEARSON(E2:E20,F2:F20)</f>
         <v>1.6108865423941535E-2</v>
       </c>
+      <c r="I2">
+        <v>0.21510000000000001</v>
+      </c>
       <c r="N2">
         <v>2766</v>
       </c>
@@ -3594,16 +3601,19 @@
         <v>1.95026469299628E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
       <c r="B3">
-        <f>8/16</f>
-        <v>0.5</v>
+        <f>10/17</f>
+        <v>0.58823529411764708</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>342</v>
@@ -3619,16 +3629,19 @@
         <v>0.81560653085512924</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
       <c r="B4">
-        <f>8/15</f>
-        <v>0.53333333333333333</v>
+        <f>10/16</f>
+        <v>0.625</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2712</v>
@@ -3644,16 +3657,19 @@
         <v>0.91196269676711517</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
       <c r="B5">
-        <f>7/13</f>
-        <v>0.53846153846153844</v>
+        <f>9/14</f>
+        <v>0.6428571428571429</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1173</v>
@@ -3669,16 +3685,16 @@
         <v>2.5364710695391026</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
       <c r="B6">
-        <f>6/12</f>
-        <v>0.5</v>
+        <f>8/13</f>
+        <v>0.61538461538461542</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>2979</v>
@@ -3694,16 +3710,19 @@
         <v>1.0112535401809375</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
       <c r="B7">
-        <f>6/11</f>
-        <v>0.54545454545454541</v>
+        <f>8/12</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1120</v>
@@ -3719,16 +3738,19 @@
         <v>1.3714423854729385</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1500</v>
       </c>
       <c r="B8">
-        <f>2/7</f>
-        <v>0.2857142857142857</v>
+        <f>4/8</f>
+        <v>0.5</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1716</v>
@@ -3744,16 +3766,19 @@
         <v>0.69641379438591922</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2000</v>
       </c>
       <c r="B9">
-        <f>2/5</f>
-        <v>0.4</v>
+        <f>4/6</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9">
         <v>1268</v>
@@ -3769,22 +3794,28 @@
         <v>1.3714423854729385</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2500</v>
       </c>
       <c r="B10">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <f>3/4</f>
+        <v>0.75</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10">
         <v>323</v>
       </c>
       <c r="F10">
         <v>0.25700000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.21729999999999999</v>
       </c>
       <c r="N10">
         <v>323</v>
@@ -3794,16 +3825,19 @@
         <v>1.182440981472024</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2900</v>
       </c>
       <c r="B11">
-        <f>0/1</f>
-        <v>0</v>
+        <f>1/1</f>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11">
         <v>181</v>
@@ -3819,7 +3853,10 @@
         <v>0.83737065613972117</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <v>181</v>
       </c>
@@ -3834,7 +3871,10 @@
         <v>0.9155865965483766</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <v>1904</v>
       </c>
@@ -3849,7 +3889,10 @@
         <v>0.9938025369570318</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <v>409</v>
       </c>
@@ -3864,7 +3907,10 @@
         <v>1.1042250410633687</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="E15">
         <v>1317</v>
       </c>
@@ -3879,7 +3925,10 @@
         <v>1.1088259787344661</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="E16">
         <v>530</v>
       </c>
@@ -3894,7 +3943,10 @@
         <v>0.84197159381081854</v>
       </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="E17">
         <v>259</v>
       </c>
@@ -3909,7 +3961,10 @@
         <v>0.74535190271777385</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="E18">
         <v>2261</v>
       </c>
@@ -3924,7 +3979,10 @@
         <v>1.219248482840803</v>
       </c>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="E19">
         <v>2627</v>
       </c>
@@ -3939,7 +3997,10 @@
         <v>1.0030044122992265</v>
       </c>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
       <c r="E20">
         <v>2412</v>
       </c>

</xml_diff>